<commit_message>
Change the letters to lowercase
Change the letters to lowercase
</commit_message>
<xml_diff>
--- a/hhnk_threedi_tools/resources/precipitation_frequency.xlsx
+++ b/hhnk_threedi_tools/resources/precipitation_frequency.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\02_Werkplaatsen\06_HYD\Projecten\HKC16015 Wateropgave 2.0\07. Poldermodellen\00.Scripts\gegevens_nabewerking\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NTNX-CIFSBEHHW01-1.corp.hhnk.nl\hydrologen_data\Data\02.modellen\heiloo_gemaal\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F69187-4489-4493-8353-EA32E5161E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,60 +27,6 @@
     <t>Ranking</t>
   </si>
   <si>
-    <t>blok_GGG_T10</t>
-  </si>
-  <si>
-    <t>blok_GGG_T100</t>
-  </si>
-  <si>
-    <t>blok_GLG_T10</t>
-  </si>
-  <si>
-    <t>blok_GLG_T100</t>
-  </si>
-  <si>
-    <t>blok_GHG_T10</t>
-  </si>
-  <si>
-    <t>blok_GHG_T100</t>
-  </si>
-  <si>
-    <t>blok_GGG_T1000</t>
-  </si>
-  <si>
-    <t>blok_GLG_T1000</t>
-  </si>
-  <si>
-    <t>blok_GHG_T1000</t>
-  </si>
-  <si>
-    <t>piek_GGG_T10</t>
-  </si>
-  <si>
-    <t>piek_GGG_T100</t>
-  </si>
-  <si>
-    <t>piek_GLG_T10</t>
-  </si>
-  <si>
-    <t>piek_GLG_T100</t>
-  </si>
-  <si>
-    <t>piek_GGG_T1000</t>
-  </si>
-  <si>
-    <t>piek_GLG_T1000</t>
-  </si>
-  <si>
-    <t>piek_GHG_T10</t>
-  </si>
-  <si>
-    <t>piek_GHG_T100</t>
-  </si>
-  <si>
-    <t>piek_GHG_T1000</t>
-  </si>
-  <si>
     <t>dl_name</t>
   </si>
   <si>
@@ -87,12 +34,66 @@
   </si>
   <si>
     <t>freq_debilt_jaar</t>
+  </si>
+  <si>
+    <t>blok_ggg_T10</t>
+  </si>
+  <si>
+    <t>piek_ggg_T10</t>
+  </si>
+  <si>
+    <t>blok_ggg_T100</t>
+  </si>
+  <si>
+    <t>blok_glg_T10</t>
+  </si>
+  <si>
+    <t>piek_ggg_T100</t>
+  </si>
+  <si>
+    <t>piek_glg_T10</t>
+  </si>
+  <si>
+    <t>blok_glg_T100</t>
+  </si>
+  <si>
+    <t>piek_glg_T100</t>
+  </si>
+  <si>
+    <t>blok_ghg_T10</t>
+  </si>
+  <si>
+    <t>blok_ghg_T100</t>
+  </si>
+  <si>
+    <t>blok_ggg_T1000</t>
+  </si>
+  <si>
+    <t>piek_ggg_T1000</t>
+  </si>
+  <si>
+    <t>blok_glg_T1000</t>
+  </si>
+  <si>
+    <t>piek_glg_T1000</t>
+  </si>
+  <si>
+    <t>piek_ghg_T10</t>
+  </si>
+  <si>
+    <t>blok_ghg_T1000</t>
+  </si>
+  <si>
+    <t>piek_ghg_T100</t>
+  </si>
+  <si>
+    <t>piek_ghg_T1000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
@@ -251,7 +252,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,7 +290,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -324,6 +325,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -359,9 +377,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -534,11 +569,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,13 +591,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -575,7 +610,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="8">
         <v>9.8309786211351127E-2</v>
@@ -594,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="8">
         <v>5.2865795391398344E-2</v>
@@ -613,7 +648,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C4" s="8">
         <v>4.3007278411203956E-2</v>
@@ -632,7 +667,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C5" s="8">
         <v>2.6678632197238553E-2</v>
@@ -651,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="8">
         <v>2.4989178894152322E-2</v>
@@ -670,7 +705,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C7" s="8">
         <v>1.7513655368832756E-2</v>
@@ -689,7 +724,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C8" s="8">
         <v>1.2299747852341175E-2</v>
@@ -708,7 +743,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8">
         <v>8.3106608069836926E-3</v>
@@ -727,7 +762,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C10" s="8">
         <v>6.0912965398784904E-3</v>
@@ -746,7 +781,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C11" s="8">
         <v>2.0360116180601433E-3</v>
@@ -765,7 +800,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C12" s="8">
         <v>1.5115102338403145E-3</v>
@@ -784,7 +819,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C13" s="8">
         <v>9.1155889995513844E-4</v>
@@ -803,7 +838,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C14" s="8">
         <v>4.6297257581990703E-4</v>
@@ -822,7 +857,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C15" s="8">
         <v>3.0373420669163321E-4</v>
@@ -841,7 +876,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C16" s="8">
         <v>1.0827642830002731E-4</v>
@@ -860,7 +895,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C17" s="8">
         <v>4.0864168793531107E-5</v>
@@ -879,7 +914,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C18" s="8">
         <v>1.9065491067081294E-5</v>
@@ -898,7 +933,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C19" s="8">
         <v>1.1875996007959881E-7</v>
@@ -926,7 +961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -938,7 +973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Klimaatsommen statistiek naar stowa verwacthing (az_dev: 25785) (#309)
* klimaatzones update

* update klimaatzones figure

* Update 03_nabewerking_klimaatsommen.py
</commit_message>
<xml_diff>
--- a/hhnk_threedi_tools/resources/precipitation_frequency.xlsx
+++ b/hhnk_threedi_tools/resources/precipitation_frequency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NTNX-CIFSBEHHW01-1.corp.hhnk.nl\hydrologen_data\Data\02.modellen\heiloo_gemaal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\Hydrologen_data\Data\github\jkaptein\hhnk-threedi-tools\hhnk_threedi_tools\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F69187-4489-4493-8353-EA32E5161E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FC897-3ACD-4B93-A4AE-9388FA67D45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,6 @@
     <t>dl_name</t>
   </si>
   <si>
-    <t>freq_hevig_jaar</t>
-  </si>
-  <si>
-    <t>freq_debilt_jaar</t>
-  </si>
-  <si>
     <t>blok_ggg_T10</t>
   </si>
   <si>
@@ -88,6 +82,12 @@
   </si>
   <si>
     <t>piek_ghg_T1000</t>
+  </si>
+  <si>
+    <t>freq_hoog_jaar</t>
+  </si>
+  <si>
+    <t>freq_referentie_jaar</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,7 +230,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -250,9 +249,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -290,9 +289,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -325,26 +324,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -377,26 +359,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -570,23 +535,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,365 +559,263 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7">
         <v>9.8309786211351127E-2</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2">
         <v>6.4573766942091895E-2</v>
       </c>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="7">
         <v>5.2865795391398344E-2</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3">
         <v>5.2865795391398344E-2</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="7">
         <v>4.3007278411203956E-2</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4">
         <v>2.615433562801088E-2</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7">
         <v>2.6678632197238553E-2</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5">
         <v>1.7839681860434116E-2</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="7">
         <v>2.4989178894152322E-2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6">
         <v>2.4989178894152322E-2</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="7">
         <v>1.7513655368832756E-2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7">
         <v>1.7513655368832756E-2</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="7">
         <v>1.2299747852341175E-2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8">
         <v>7.5836886888358155E-3</v>
       </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7">
         <v>8.3106608069836926E-3</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9">
         <v>8.3106608069836926E-3</v>
       </c>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="7">
         <v>6.0912965398784904E-3</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10">
         <v>3.6849071202631834E-3</v>
       </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7">
         <v>2.0360116180601433E-3</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11">
         <v>1.1344231871678113E-3</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="7">
         <v>1.5115102338403145E-3</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12">
         <v>7.8896861831863373E-4</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7">
         <v>9.1155889995513844E-4</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13">
         <v>9.1155889995513844E-4</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="7">
         <v>4.6297257581990703E-4</v>
       </c>
-      <c r="D14" s="7">
+      <c r="D14">
         <v>2.4360700079881445E-4</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C15" s="8">
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="7">
         <v>3.0373420669163321E-4</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15">
         <v>3.0373420669163321E-4</v>
       </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="7">
         <v>1.0827642830002731E-4</v>
       </c>
-      <c r="D16" s="7">
+      <c r="D16">
         <v>1.0827642830002731E-4</v>
       </c>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="8">
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="7">
         <v>4.0864168793531107E-5</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17">
         <v>1.9382538640730108E-5</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="7">
         <v>1.9065491067081294E-5</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18">
         <v>1.9065491067081294E-5</v>
       </c>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="7">
         <v>1.1875996007959881E-7</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19">
         <v>1.1875996007959881E-7</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -966,7 +829,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -978,7 +841,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' into Vergelijkingstool"
This reverts commit 75dad5ae0a5e6505e8f80edc286f83445aabcf9a, reversing
changes made to 92873fb44d1a4851bb483475852bb98d7f458cf3.
</commit_message>
<xml_diff>
--- a/hhnk_threedi_tools/resources/precipitation_frequency.xlsx
+++ b/hhnk_threedi_tools/resources/precipitation_frequency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.hhnk.nl\data\Hydrologen_data\Data\github\jkaptein\hhnk-threedi-tools\hhnk_threedi_tools\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\NTNX-CIFSBEHHW01-1.corp.hhnk.nl\hydrologen_data\Data\02.modellen\heiloo_gemaal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE5FC897-3ACD-4B93-A4AE-9388FA67D45F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F69187-4489-4493-8353-EA32E5161E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,6 +30,12 @@
     <t>dl_name</t>
   </si>
   <si>
+    <t>freq_hevig_jaar</t>
+  </si>
+  <si>
+    <t>freq_debilt_jaar</t>
+  </si>
+  <si>
     <t>blok_ggg_T10</t>
   </si>
   <si>
@@ -82,12 +88,6 @@
   </si>
   <si>
     <t>piek_ghg_T1000</t>
-  </si>
-  <si>
-    <t>freq_hoog_jaar</t>
-  </si>
-  <si>
-    <t>freq_referentie_jaar</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -230,6 +230,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -249,9 +250,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -289,9 +290,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,9 +325,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -359,9 +377,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -535,23 +570,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,263 +594,365 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="B2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8">
         <v>9.8309786211351127E-2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="7">
         <v>6.4573766942091895E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8">
         <v>5.2865795391398344E-2</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="7">
         <v>5.2865795391398344E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8">
         <v>4.3007278411203956E-2</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="7">
         <v>2.615433562801088E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="7">
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="8">
         <v>2.6678632197238553E-2</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="7">
         <v>1.7839681860434116E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8">
         <v>2.4989178894152322E-2</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="7">
         <v>2.4989178894152322E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="7">
+      <c r="B7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8">
         <v>1.7513655368832756E-2</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="7">
         <v>1.7513655368832756E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="8">
         <v>1.2299747852341175E-2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="7">
         <v>7.5836886888358155E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="7">
+      <c r="B9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="8">
         <v>8.3106608069836926E-3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="7">
         <v>8.3106608069836926E-3</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="B10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="8">
         <v>6.0912965398784904E-3</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="7">
         <v>3.6849071202631834E-3</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7">
+      <c r="B11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="8">
         <v>2.0360116180601433E-3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>1.1344231871678113E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="8">
         <v>1.5115102338403145E-3</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>7.8896861831863373E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="8">
         <v>9.1155889995513844E-4</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>9.1155889995513844E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="7">
+      <c r="B14" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="8">
         <v>4.6297257581990703E-4</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>2.4360700079881445E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="7">
+      <c r="B15" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="8">
         <v>3.0373420669163321E-4</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>3.0373420669163321E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="7">
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="8">
         <v>1.0827642830002731E-4</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="7">
         <v>1.0827642830002731E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="7">
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8">
         <v>4.0864168793531107E-5</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7">
         <v>1.9382538640730108E-5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="B18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="8">
         <v>1.9065491067081294E-5</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="7">
         <v>1.9065491067081294E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="7">
+      <c r="B19" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="8">
         <v>1.1875996007959881E-7</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>1.1875996007959881E-7</v>
       </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -829,7 +966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -841,7 +978,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>